<commit_message>
added plot for prospective insights
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanhachez/Documents/ongoing - DHN_expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="115_{FF50BDCB-5647-44AE-A376-5FC91899235D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02879FB9-7A4A-4216-A814-74FEF31E32F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E18FA24-02D6-344A-99AF-A8C6A582823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-67260" yWindow="-5320" windowWidth="26640" windowHeight="19800" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>parameter</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>multiplier</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>Pit</t>
   </si>
 </sst>
 </file>
@@ -211,9 +217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -251,7 +257,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -357,7 +363,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,9 +517,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -529,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -537,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -545,7 +554,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -553,7 +562,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -561,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -569,7 +578,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -577,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -585,7 +594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -602,26 +611,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0E9847-B35B-42F7-B80E-8901083A9132}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.58203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -656,7 +665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -691,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -726,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -761,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -803,97 +812,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B9AB8C-FEEB-44DF-BE7F-AAE13A717E9E}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>25000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
+      <c r="C2">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
+      <c r="D2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
+      <c r="E2">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
+      <c r="F2">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
+      <c r="G2">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8">
+      <c r="H2">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9">
+      <c r="I2">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10">
+      <c r="J2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
+      <c r="K2">
         <v>0</v>
       </c>
     </row>
@@ -908,9 +913,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -918,7 +926,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -926,7 +934,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -934,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -953,9 +961,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -963,7 +974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -971,7 +982,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -979,7 +990,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -987,7 +998,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1006,9 +1017,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1024,7 +1038,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1032,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
simulation finished - working on outputs
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanhachez/Documents/ongoing - DHN_expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E18FA24-02D6-344A-99AF-A8C6A582823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683A5AEC-B063-E54C-9423-1B50F033F882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67260" yWindow="-5320" windowWidth="26640" windowHeight="19800" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="3220" yWindow="760" windowWidth="26640" windowHeight="17680" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>parameter</t>
   </si>
@@ -132,12 +132,6 @@
   </si>
   <si>
     <t>max_discharge_rate</t>
-  </si>
-  <si>
-    <t>lifetime</t>
-  </si>
-  <si>
-    <t>max_capacity</t>
   </si>
   <si>
     <t>carrier</t>
@@ -612,7 +606,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B9AB8C-FEEB-44DF-BE7F-AAE13A717E9E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -858,10 +852,10 @@
         <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
@@ -869,7 +863,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>25000</v>
@@ -911,7 +905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45E1C8F-A0B8-43F8-85A1-21F7CD6ECE72}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -920,10 +916,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -968,10 +964,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1024,10 +1020,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update model parameters in Excel file
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="498" documentId="11_C06996C0FE411BF93D0577E108B2978BCD23EF9B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED2CC54-199E-4AA1-BEC6-FABFBEF61C72}"/>
+  <xr:revisionPtr revIDLastSave="531" documentId="11_C06996C0FE411BF93D0577E108B2978BCD23EF9B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E03A74F-185D-442F-9E53-ABE94CA8220D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -45,6 +45,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={98EB3A2A-984A-4989-8252-77BD7D530C82}</author>
+    <author>tc={2B9DC85E-C269-467E-AAB3-45AA130E6B73}</author>
+    <author>tc={B7D506CE-A6BB-470A-875D-9FA84DE22FB9}</author>
   </authors>
   <commentList>
     <comment ref="C2" authorId="0" shapeId="0" xr:uid="{98EB3A2A-984A-4989-8252-77BD7D530C82}">
@@ -55,12 +57,28 @@
     EUR values converted to SEK by multiplying by 10,92</t>
       </text>
     </comment>
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{2B9DC85E-C269-467E-AAB3-45AA130E6B73}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Increase</t>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="2" shapeId="0" xr:uid="{B7D506CE-A6BB-470A-875D-9FA84DE22FB9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Late increase</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>multiplier</t>
   </si>
@@ -303,6 +321,9 @@
   </si>
   <si>
     <t>bio_waste</t>
+  </si>
+  <si>
+    <t>use_stochastic_demand</t>
   </si>
 </sst>
 </file>
@@ -343,12 +364,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -371,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -406,6 +433,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,6 +753,12 @@
   <threadedComment ref="C2" dT="2025-10-24T14:22:12.17" personId="{225DE312-2597-4284-8E1A-4635D93CA1E7}" id="{98EB3A2A-984A-4989-8252-77BD7D530C82}">
     <text>EUR values converted to SEK by multiplying by 10,92</text>
   </threadedComment>
+  <threadedComment ref="B3" dT="2025-10-28T09:22:43.82" personId="{225DE312-2597-4284-8E1A-4635D93CA1E7}" id="{2B9DC85E-C269-467E-AAB3-45AA130E6B73}">
+    <text>Increase</text>
+  </threadedComment>
+  <threadedComment ref="B4" dT="2025-10-28T09:22:51.08" personId="{225DE312-2597-4284-8E1A-4635D93CA1E7}" id="{B7D506CE-A6BB-470A-875D-9FA84DE22FB9}">
+    <text>Late increase</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -726,15 +767,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -819,6 +860,14 @@
       </c>
       <c r="C8" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -834,7 +883,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,8 +948,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,7 +957,7 @@
     <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.90625" style="4" bestFit="1" customWidth="1"/>
@@ -1265,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1300,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1426,7 +1475,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1491,12 +1540,13 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="23.81640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.90625" style="12"/>
   </cols>
   <sheetData>
@@ -1745,7 +1795,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1753,10 +1803,10 @@
     <col min="1" max="1" width="5.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1769,7 +1819,7 @@
       <c r="C1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="16" t="s">
         <v>69</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -1792,9 +1842,9 @@
       <c r="C2">
         <v>2023</v>
       </c>
-      <c r="D2">
-        <f>D3*1.15</f>
-        <v>-1449</v>
+      <c r="D2" s="17">
+        <f>D3*0.75</f>
+        <v>-945</v>
       </c>
       <c r="E2">
         <f>E3*1.3</f>
@@ -1805,8 +1855,8 @@
         <v>304.2</v>
       </c>
       <c r="G2">
-        <f>G3*1.15</f>
-        <v>740.59999999999991</v>
+        <f>G3*1.3</f>
+        <v>837.2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1819,7 +1869,7 @@
       <c r="C3">
         <v>2023</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="18">
         <v>-1260</v>
       </c>
       <c r="E3">
@@ -1842,9 +1892,9 @@
       <c r="C4">
         <v>2023</v>
       </c>
-      <c r="D4">
-        <f>D3*0.85</f>
-        <v>-1071</v>
+      <c r="D4" s="17">
+        <f>D3*1.15</f>
+        <v>-1449</v>
       </c>
       <c r="E4">
         <f>E3*0.7</f>
@@ -1855,8 +1905,8 @@
         <v>163.79999999999998</v>
       </c>
       <c r="G4">
-        <f>G3*0.85</f>
-        <v>547.4</v>
+        <f>G3*0.7</f>
+        <v>450.79999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1869,9 +1919,9 @@
       <c r="C5">
         <v>2030</v>
       </c>
-      <c r="D5">
-        <f>D6*1.15</f>
-        <v>-1838.85</v>
+      <c r="D5" s="17">
+        <f>D6*0.75</f>
+        <v>-1199.25</v>
       </c>
       <c r="E5">
         <f>E6*1.3</f>
@@ -1882,8 +1932,8 @@
         <v>341.90000000000003</v>
       </c>
       <c r="G5">
-        <f>G6*1.15</f>
-        <v>832.59999999999991</v>
+        <f>G6*1.3</f>
+        <v>941.2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1896,7 +1946,7 @@
       <c r="C6">
         <v>2030</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="18">
         <v>-1599</v>
       </c>
       <c r="E6">
@@ -1919,9 +1969,9 @@
       <c r="C7">
         <v>2030</v>
       </c>
-      <c r="D7">
-        <f>D6*0.85</f>
-        <v>-1359.1499999999999</v>
+      <c r="D7" s="17">
+        <f>D6*1.15</f>
+        <v>-1838.85</v>
       </c>
       <c r="E7">
         <f>E6*0.7</f>
@@ -1932,8 +1982,8 @@
         <v>184.1</v>
       </c>
       <c r="G7">
-        <f>G6*0.85</f>
-        <v>615.4</v>
+        <f>G6*0.7</f>
+        <v>506.79999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1946,9 +1996,9 @@
       <c r="C8">
         <v>2040</v>
       </c>
-      <c r="D8">
-        <f>D9*1.15</f>
-        <v>-2285.0499999999997</v>
+      <c r="D8" s="17">
+        <f>D9*0.75</f>
+        <v>-1490.25</v>
       </c>
       <c r="E8">
         <f>E9*1.3</f>
@@ -1959,8 +2009,8 @@
         <v>403</v>
       </c>
       <c r="G8">
-        <f>G9*1.15</f>
-        <v>985.55</v>
+        <f>G9*1.3</f>
+        <v>1114.1000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1973,7 +2023,7 @@
       <c r="C9">
         <v>2040</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="18">
         <v>-1987</v>
       </c>
       <c r="E9">
@@ -1996,9 +2046,9 @@
       <c r="C10">
         <v>2040</v>
       </c>
-      <c r="D10">
-        <f>D9*0.85</f>
-        <v>-1688.95</v>
+      <c r="D10" s="17">
+        <f>D9*1.15</f>
+        <v>-2285.0499999999997</v>
       </c>
       <c r="E10">
         <f>E9*0.7</f>
@@ -2009,8 +2059,8 @@
         <v>217</v>
       </c>
       <c r="G10">
-        <f>G9*0.85</f>
-        <v>728.44999999999993</v>
+        <f>G9*0.7</f>
+        <v>599.9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2023,9 +2073,9 @@
       <c r="C11">
         <v>2050</v>
       </c>
-      <c r="D11">
-        <f>D12*1.15</f>
-        <v>-2619.6999999999998</v>
+      <c r="D11" s="17">
+        <f>D12*0.75</f>
+        <v>-1708.5</v>
       </c>
       <c r="E11">
         <f>E12*1.3</f>
@@ -2036,8 +2086,8 @@
         <v>477.1</v>
       </c>
       <c r="G11">
-        <f>G12*1.15</f>
-        <v>1167.25</v>
+        <f>G12*1.3</f>
+        <v>1319.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2050,7 +2100,7 @@
       <c r="C12">
         <v>2050</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="18">
         <v>-2278</v>
       </c>
       <c r="E12">
@@ -2073,9 +2123,9 @@
       <c r="C13">
         <v>2050</v>
       </c>
-      <c r="D13">
-        <f>D12*0.85</f>
-        <v>-1936.3</v>
+      <c r="D13" s="17">
+        <f>D12*1.15</f>
+        <v>-2619.6999999999998</v>
       </c>
       <c r="E13">
         <f>E12*0.7</f>
@@ -2086,8 +2136,8 @@
         <v>256.89999999999998</v>
       </c>
       <c r="G13">
-        <f>G12*0.85</f>
-        <v>862.75</v>
+        <f>G12*0.7</f>
+        <v>710.5</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +2153,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2181,7 +2231,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2285,7 +2335,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Rename CarbonTrajectories sheet to CarbonTrajectory
Fix sheet name to match singular form used in parameters.jl code.
This resolves the 'not a valid sheetname' error during parameter loading.
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="115_{9A63A160-9015-40FE-AA27-35B1EC3B8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{674B3A12-EEB7-4E27-9080-CE7C6F0D2D84}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="115_{9A63A160-9015-40FE-AA27-35B1EC3B8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7735B41-8BF4-455E-BBA8-58B267DA211C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="7" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="10" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="EnergyPriceMap" sheetId="7" r:id="rId7"/>
     <sheet name="EnergyTransitions" sheetId="8" r:id="rId8"/>
     <sheet name="DemandUncertainty" sheetId="9" r:id="rId9"/>
-    <sheet name="CarbonTrajectories" sheetId="10" r:id="rId10"/>
+    <sheet name="CarbonTrajectory" sheetId="10" r:id="rId10"/>
     <sheet name="TemperatureScenarios" sheetId="11" r:id="rId11"/>
     <sheet name="TemperatureProbabilities" sheetId="12" r:id="rId12"/>
     <sheet name="ExistingCapacitySchedule" sheetId="13" r:id="rId13"/>
@@ -704,9 +704,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -747,7 +747,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -758,7 +758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -777,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -805,11 +805,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B137F6-4E69-4E75-88FC-D51AC0D90317}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -823,7 +825,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1500</v>
       </c>
@@ -846,16 +848,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE9921C-EC1D-48DB-9CE9-5FEAD03EEB74}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -866,7 +868,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -877,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -899,9 +901,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -912,7 +914,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -923,7 +925,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -945,9 +947,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -964,7 +966,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -981,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1015,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1049,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1145,9 +1147,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1161,7 +1163,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.81120000000000003</v>
       </c>
@@ -1186,9 +1188,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7657579.3700000001</v>
       </c>
@@ -1227,14 +1229,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1269,7 +1271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1444,7 +1446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1479,7 +1481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1549,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1630,9 +1632,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1649,7 +1651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1666,7 +1668,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1700,7 +1702,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1717,7 +1719,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1734,7 +1736,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1768,7 +1770,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1785,7 +1787,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1819,7 +1821,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1847,9 +1849,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1873,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1881,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1889,7 +1891,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1905,7 +1907,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1929,7 +1931,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1948,9 +1950,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1958,7 +1960,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1966,7 +1968,7 @@
         <v>0.34735402116783071</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1974,12 +1976,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2006,9 +2008,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2016,7 +2018,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -2024,7 +2026,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -2040,7 +2042,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2048,7 +2050,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -2056,7 +2058,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -2072,7 +2074,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -2096,7 +2098,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -2136,7 +2138,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -2160,7 +2162,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -2168,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -2176,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -2184,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -2200,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -2208,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -2216,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -2253,18 +2255,18 @@
       <selection activeCell="E11" sqref="E11:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2310,7 +2312,7 @@
         <v>837.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>450.79999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2379,7 +2381,7 @@
         <v>941.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -2402,7 +2404,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2425,7 +2427,7 @@
         <v>506.79999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2448,7 +2450,7 @@
         <v>1114.1000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>599.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2517,7 +2519,7 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2572,13 +2574,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D179FE01-73A4-4F8D-AE11-2B1C5DCF85D7}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -2592,7 +2594,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
@@ -2606,7 +2608,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -2645,9 +2647,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -2658,7 +2660,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1.05</v>
       </c>
@@ -2669,7 +2671,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2680,7 +2682,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.95</v>
       </c>

</xml_diff>

<commit_message>
Implement extreme events as stage-wise independent uncertainty
Add configurable extreme events feature to model severe disruptions at specific operational stages. Events can modify demand, electricity prices, and data center availability simultaneously.

- Load ExtremeEventControl and ExtremeEvents sheets from Excel
- Apply extreme event scenarios via SDDP.parameterize at specified stage
- Integrate expected values into deterministic benchmark model
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="115_{9A63A160-9015-40FE-AA27-35B1EC3B8FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7735B41-8BF4-455E-BBA8-58B267DA211C}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E6DB9A-53C1-435D-BBD5-A56E02019541}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="10" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="6" activeTab="8" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Emission_Factor_for_electricity" sheetId="6" r:id="rId6"/>
     <sheet name="EnergyPriceMap" sheetId="7" r:id="rId7"/>
     <sheet name="EnergyTransitions" sheetId="8" r:id="rId8"/>
-    <sheet name="DemandUncertainty" sheetId="9" r:id="rId9"/>
-    <sheet name="CarbonTrajectory" sheetId="10" r:id="rId10"/>
-    <sheet name="TemperatureScenarios" sheetId="11" r:id="rId11"/>
-    <sheet name="TemperatureProbabilities" sheetId="12" r:id="rId12"/>
-    <sheet name="ExistingCapacitySchedule" sheetId="13" r:id="rId13"/>
-    <sheet name="WasteChpEfficiency" sheetId="14" r:id="rId14"/>
-    <sheet name="WasteAvailability" sheetId="15" r:id="rId15"/>
+    <sheet name="CarbonTrajectory" sheetId="10" r:id="rId9"/>
+    <sheet name="TemperatureScenarios" sheetId="11" r:id="rId10"/>
+    <sheet name="TemperatureProbabilities" sheetId="12" r:id="rId11"/>
+    <sheet name="ExistingCapacitySchedule" sheetId="13" r:id="rId12"/>
+    <sheet name="WasteChpEfficiency" sheetId="14" r:id="rId13"/>
+    <sheet name="WasteAvailability" sheetId="15" r:id="rId14"/>
+    <sheet name="ExtremeEvents" sheetId="16" r:id="rId15"/>
+    <sheet name="ExtremeEventControl" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="107">
   <si>
     <t>parameter</t>
   </si>
@@ -263,21 +264,9 @@
     <t>to_low</t>
   </si>
   <si>
-    <t>multiplier</t>
-  </si>
-  <si>
     <t>probability</t>
   </si>
   <si>
-    <t>High demand</t>
-  </si>
-  <si>
-    <t>Normal demand</t>
-  </si>
-  <si>
-    <t>Low demand</t>
-  </si>
-  <si>
     <t>year_1[SEK/tCO2]</t>
   </si>
   <si>
@@ -312,6 +301,66 @@
   </si>
   <si>
     <t>year_4</t>
+  </si>
+  <si>
+    <t>elec_price_multiplier</t>
+  </si>
+  <si>
+    <t>dc_availability</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>demand_surge</t>
+  </si>
+  <si>
+    <t>price_spike</t>
+  </si>
+  <si>
+    <t>dc_outage</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal - baseline conditions  </t>
+  </si>
+  <si>
+    <t>Climate stress - more severe winters (20% higher average demand)</t>
+  </si>
+  <si>
+    <t>Energy crisis  -  high electricity prices (2x average)</t>
+  </si>
+  <si>
+    <t>Data center supply distruption  - complete unavailability</t>
+  </si>
+  <si>
+    <t>enable_extreme_events</t>
+  </si>
+  <si>
+    <t>apply_to_year</t>
+  </si>
+  <si>
+    <t>Master switch to enable/disable extreme event modeling</t>
+  </si>
+  <si>
+    <t>Which model year to apply extreme events</t>
+  </si>
+  <si>
+    <t>demand_multiplier</t>
   </si>
 </sst>
 </file>
@@ -699,14 +748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA425C3-2FB2-49C0-BE7B-8EE127A81638}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590D77B-7759-431A-924A-4D4114C0C169}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -728,7 +777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -739,7 +788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -747,7 +796,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -758,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -766,7 +815,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -777,7 +826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -788,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -802,41 +851,49 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B137F6-4E69-4E75-88FC-D51AC0D90317}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916A681A-3E86-4F06-B784-91FE6167CDD3}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>79</v>
       </c>
       <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1500</v>
-      </c>
-      <c r="B2">
-        <v>1900</v>
-      </c>
-      <c r="C2">
-        <v>2300</v>
-      </c>
-      <c r="D2">
-        <v>2730</v>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -845,49 +902,44 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE9921C-EC1D-48DB-9CE9-5FEAD03EEB74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22286C85-1058-4683-BC8D-55516C17C647}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -896,44 +948,198 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D936589-D958-4516-8E81-3A62176292EB}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145D0F8-96F7-4B36-9ED7-5DAF3228EE46}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
       <c r="C1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>85</v>
       </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>192.71</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>220</v>
+      </c>
+      <c r="C5">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>517.29</v>
+      </c>
+      <c r="C6">
+        <v>444.3</v>
+      </c>
+      <c r="D6">
+        <v>227.7</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>314.57</v>
+      </c>
+      <c r="C8">
+        <v>78</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>185</v>
+      </c>
+      <c r="C9">
+        <v>102</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1702.14</v>
+      </c>
+      <c r="C10">
+        <v>861.2</v>
+      </c>
+      <c r="D10">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>333</v>
+      </c>
+      <c r="C11">
+        <v>274.5</v>
+      </c>
+      <c r="D11">
+        <v>55.9</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -942,198 +1148,39 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7B8642-CB04-4C66-8DC5-30F64C991194}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF04874-5E52-4CAF-80BF-0F4F010E9C18}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0.81120000000000003</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.63560000000000005</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.53320000000000001</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3">
-        <v>192.71</v>
-      </c>
-      <c r="C3">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>220</v>
-      </c>
-      <c r="C5">
-        <v>66</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>517.29</v>
-      </c>
-      <c r="C6">
-        <v>444.3</v>
-      </c>
-      <c r="D6">
-        <v>227.7</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>314.57</v>
-      </c>
-      <c r="C8">
-        <v>78</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>185</v>
-      </c>
-      <c r="C9">
-        <v>102</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10">
-        <v>1702.14</v>
-      </c>
-      <c r="C10">
-        <v>861.2</v>
-      </c>
-      <c r="D10">
-        <v>56</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11">
-        <v>333</v>
-      </c>
-      <c r="C11">
-        <v>274.5</v>
-      </c>
-      <c r="D11">
-        <v>55.9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>0.49769999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1142,39 +1189,39 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9F920B-16FB-4393-9856-AF142B016095}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA441E4D-3EA7-459F-85DE-ECA5E8A27D8A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.81120000000000003</v>
+        <v>7657579.3700000001</v>
       </c>
       <c r="B2">
-        <v>0.63560000000000005</v>
+        <v>5474361.1100000003</v>
       </c>
       <c r="C2">
-        <v>0.53320000000000001</v>
+        <v>3731500</v>
       </c>
       <c r="D2">
-        <v>0.49769999999999998</v>
+        <v>3034115.53</v>
       </c>
     </row>
   </sheetData>
@@ -1183,39 +1230,172 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92A63BD-08BF-48B4-8775-74AC8131084F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0160E0F-AD26-48ED-8931-1C59DFE62250}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4035866-F30E-4239-8029-E32D08CAEEBA}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>7657579.3700000001</v>
-      </c>
-      <c r="B2">
-        <v>5474361.1100000003</v>
-      </c>
-      <c r="C2">
-        <v>3731500</v>
-      </c>
-      <c r="D2">
-        <v>3034115.53</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1224,19 +1404,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EDAEEE-57BE-437F-AD35-40710465E339}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B221ABC6-770B-4F46-8362-7A6F0CE97577}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1341,7 +1521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1376,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1446,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1481,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1516,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1551,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1586,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1627,14 +1807,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144BCC24-8A69-4996-B30C-614672110C9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420D5219-3D62-48D2-B079-889AEB0D6350}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1651,7 +1833,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1668,7 +1850,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1685,7 +1867,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1702,7 +1884,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1719,7 +1901,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1736,7 +1918,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1753,7 +1935,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1770,7 +1952,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1787,7 +1969,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1804,7 +1986,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1821,7 +2003,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1844,14 +2026,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33051478-F6D3-4475-8480-F2CF825CE378}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E078A6-3DE3-4FBD-B546-0DA5EF096AA6}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1867,7 +2049,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1875,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1883,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1891,7 +2073,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1899,7 +2081,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1907,7 +2089,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1915,7 +2097,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1923,7 +2105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1931,7 +2113,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1945,14 +2127,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD4047E-AB93-4DC5-B789-053BA65F46B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C4674D-613B-47DC-95EC-A125610F3DBD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1960,7 +2142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1968,7 +2150,7 @@
         <v>0.34735402116783071</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1976,12 +2158,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1989,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2003,14 +2185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8B9343-7A8D-46EB-B401-069B95278156}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03C60C6-D733-44AF-9BC0-050CCF024BCE}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2018,7 +2200,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -2026,7 +2208,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -2034,7 +2216,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -2042,7 +2224,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2050,7 +2232,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -2058,7 +2240,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -2066,7 +2248,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -2074,7 +2256,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -2082,7 +2264,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -2090,7 +2272,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -2098,7 +2280,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -2106,7 +2288,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -2114,7 +2296,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -2122,7 +2304,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -2130,7 +2312,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -2138,7 +2320,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -2146,7 +2328,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -2154,7 +2336,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -2162,7 +2344,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -2170,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -2178,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -2186,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -2194,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -2202,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -2210,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -2218,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -2226,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -2234,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -2248,25 +2430,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01227A19-DAA9-40BA-8159-509A46C35B21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE8A0B0-FF39-49E0-ADEA-C8C600021327}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E11" sqref="E11:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2289,7 +2471,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2312,7 +2494,7 @@
         <v>837.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2335,7 +2517,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2358,7 +2540,7 @@
         <v>450.79999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2381,7 +2563,7 @@
         <v>941.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -2404,7 +2586,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2427,7 +2609,7 @@
         <v>506.79999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2450,7 +2632,7 @@
         <v>1114.1000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -2473,7 +2655,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -2496,7 +2678,7 @@
         <v>599.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2519,7 +2701,7 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -2542,7 +2724,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2571,16 +2753,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D179FE01-73A4-4F8D-AE11-2B1C5DCF85D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879CF66E-0559-4CA6-9CC7-E6C1E475771D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -2594,7 +2776,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
@@ -2608,7 +2790,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
@@ -2622,7 +2804,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
@@ -2642,55 +2824,41 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E25F9-B4AF-4660-B439-978F43A19A38}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51FC39B-AAD9-4476-8BBF-DA36EB745D6A}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1.05</v>
+        <v>1500</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.95</v>
-      </c>
-      <c r="B4">
-        <v>0.2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
+        <v>1900</v>
+      </c>
+      <c r="C2">
+        <v>2300</v>
+      </c>
+      <c r="D2">
+        <v>2730</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unused demand uncertainty implementation
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E6DB9A-53C1-435D-BBD5-A56E02019541}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{023C3E1A-02F7-4ADD-91D3-56A17B208543}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="6" activeTab="8" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="106">
   <si>
     <t>parameter</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>elec_taxes_levies</t>
-  </si>
-  <si>
-    <t>use_stochastic_demand</t>
   </si>
   <si>
     <t>technology</t>
@@ -749,11 +746,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590D77B-7759-431A-924A-4D4114C0C169}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -835,14 +838,6 @@
       </c>
       <c r="C8" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -865,13 +860,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -879,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -890,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -911,13 +906,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -925,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -936,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -957,24 +952,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -991,7 +986,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>192.71</v>
@@ -1008,7 +1003,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1025,7 +1020,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>220</v>
@@ -1042,7 +1037,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>517.29</v>
@@ -1059,7 +1054,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1076,7 +1071,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>314.57</v>
@@ -1093,7 +1088,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>185</v>
@@ -1110,7 +1105,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>1702.14</v>
@@ -1127,7 +1122,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>333</v>
@@ -1157,16 +1152,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1198,16 +1193,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1249,30 +1244,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1284,18 +1279,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1304,15 +1299,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1324,15 +1319,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1344,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1373,29 +1368,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1418,42 +1413,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>330</v>
@@ -1477,7 +1472,7 @@
         <v>0.26</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -1488,7 +1483,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>430</v>
@@ -1512,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1523,7 +1518,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>320</v>
@@ -1547,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1558,7 +1553,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>185</v>
@@ -1582,7 +1577,7 @@
         <v>0.21</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -1593,7 +1588,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>522</v>
@@ -1617,7 +1612,7 @@
         <v>0.27</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -1628,7 +1623,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>1700</v>
@@ -1652,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1663,7 +1658,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>275</v>
@@ -1687,7 +1682,7 @@
         <v>0.5</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -1698,7 +1693,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1722,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -1733,7 +1728,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>220</v>
@@ -1757,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -1768,7 +1763,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1792,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -1818,24 +1813,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>-1</v>
@@ -1852,7 +1847,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -1869,7 +1864,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -1886,7 +1881,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -1903,7 +1898,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -1920,7 +1915,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -1937,7 +1932,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -1954,7 +1949,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -1971,7 +1966,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -1988,7 +1983,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -2005,7 +2000,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -2043,7 +2038,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>400</v>
@@ -2051,7 +2046,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2059,7 +2054,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2067,7 +2062,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>0.95</v>
@@ -2075,7 +2070,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.02</v>
@@ -2083,7 +2078,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>0.25</v>
@@ -2091,7 +2086,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.25</v>
@@ -2099,7 +2094,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2107,7 +2102,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>1000</v>
@@ -2115,7 +2110,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2136,15 +2131,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.34735402116783071</v>
@@ -2152,7 +2147,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2160,12 +2155,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2173,7 +2168,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2194,10 +2189,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2450,25 +2445,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2476,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1">
         <v>2023</v>
@@ -2499,7 +2494,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
         <v>2023</v>
@@ -2522,7 +2517,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1">
         <v>2023</v>
@@ -2545,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2">
         <v>2030</v>
@@ -2568,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4">
         <v>2030</v>
@@ -2591,7 +2586,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2">
         <v>2030</v>
@@ -2614,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3">
         <v>2040</v>
@@ -2637,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4">
         <v>2040</v>
@@ -2660,7 +2655,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3">
         <v>2040</v>
@@ -2683,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>2050</v>
@@ -2706,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4">
         <v>2050</v>
@@ -2729,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>2050</v>
@@ -2764,21 +2759,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>0.6</v>
@@ -2792,7 +2787,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -2806,7 +2801,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -2827,7 +2822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51FC39B-AAD9-4476-8BBF-DA36EB745D6A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2835,16 +2830,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add temperature-dependent demand multiplier and fix Markov chain initial state
- Add temp_demand_multipliers to ModelParameters for scenario-specific demand scaling
- Load demand_multiplier from TemperatureScenarios Excel sheet (defaults to 1.0)
- Apply temperature demand multiplier to demand constraint in model_builder
- Fix initial_energy_dist to use Medium state row from transition matrix
  (ensures consistency with Markov chain dynamics instead of arbitrary [0.3, 0.4, 0.3])
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{023C3E1A-02F7-4ADD-91D3-56A17B208543}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C832D6-4F70-4BB5-8EAC-77EEFB19A4E5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>parameter</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>demand_multiplier</t>
+  </si>
+  <si>
+    <t>0.8</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -774,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -785,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -847,10 +850,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916A681A-3E86-4F06-B784-91FE6167CDD3}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -858,7 +861,7 @@
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -868,8 +871,11 @@
       <c r="C1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -879,8 +885,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -889,6 +898,9 @@
       </c>
       <c r="C3">
         <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -900,7 +912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22286C85-1058-4683-BC8D-55516C17C647}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -946,9 +960,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145D0F8-96F7-4B36-9ED7-5DAF3228EE46}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1229,7 +1248,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1402,7 +1421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B221ABC6-770B-4F46-8362-7A6F0CE97577}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2024,9 +2045,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E078A6-3DE3-4FBD-B546-0DA5EF096AA6}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2428,15 +2455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE8A0B0-FF39-49E0-ADEA-C8C600021327}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
@@ -2776,13 +2803,13 @@
         <v>66</v>
       </c>
       <c r="B2">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.09</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2790,13 +2817,13 @@
         <v>67</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2804,13 +2831,13 @@
         <v>68</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
-        <v>0.3</v>
+        <v>0.09</v>
       </c>
       <c r="D4">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -2823,10 +2850,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
modified typical days for Ali
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanhachez/Documents/ongoing - DHN_expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B9ECC-149D-414E-9575-3D267969635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD985E33-6DEC-3847-B90A-E26701D7D4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="18" r:id="rId1"/>
@@ -3303,7 +3303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E523C0-40CD-474E-8EE1-DF88A4494E55}">
   <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+    <sheetView topLeftCell="A147" workbookViewId="0">
       <selection activeCell="G162" sqref="G162"/>
     </sheetView>
   </sheetViews>
@@ -8349,8 +8349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B13672-FC01-1744-AF2E-411812A2A98C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactor data loading for scenario-specific demand and electricity prices
- Load demand and prices from unified typical_weeks_{n}.csv file
- Demand now varies by energy price scenario (high/medium/low) per year
- ProcessedData.scaled_weeks structure changed: Dict{Int, Dict{Symbol, Vector{Vector{Float64}}}}
- Add n_typical_weeks parameter for configurable representative weeks
- Add calendar year mapping (2023, 2030, 2035/2040, etc.) for Excel columns
- Year-varying temperature demand multipliers (vector per scenario)
- Remove lifetime_initial (use ExistingCapacitySchedule only)
- Scale lifetime_new based on T_years for flexibility
- Convert waste availability from GWh to MWh
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="115_{34DC912F-EE65-44D9-9C9B-3B52B854FD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C832D6-4F70-4BB5-8EAC-77EEFB19A4E5}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF1C899-01B6-4747-A846-150BBD65C624}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -21,26 +21,53 @@
     <sheet name="Emission_Factor_for_electricity" sheetId="6" r:id="rId6"/>
     <sheet name="EnergyPriceMap" sheetId="7" r:id="rId7"/>
     <sheet name="EnergyTransitions" sheetId="8" r:id="rId8"/>
-    <sheet name="CarbonTrajectory" sheetId="10" r:id="rId9"/>
-    <sheet name="TemperatureScenarios" sheetId="11" r:id="rId10"/>
-    <sheet name="TemperatureProbabilities" sheetId="12" r:id="rId11"/>
-    <sheet name="ExistingCapacitySchedule" sheetId="13" r:id="rId12"/>
-    <sheet name="WasteChpEfficiency" sheetId="14" r:id="rId13"/>
-    <sheet name="WasteAvailability" sheetId="15" r:id="rId14"/>
-    <sheet name="ExtremeEvents" sheetId="16" r:id="rId15"/>
-    <sheet name="ExtremeEventControl" sheetId="17" r:id="rId16"/>
+    <sheet name="CarbonTrajectory" sheetId="9" r:id="rId9"/>
+    <sheet name="TemperatureScenarios" sheetId="10" r:id="rId10"/>
+    <sheet name="TemperatureProbabilities" sheetId="11" r:id="rId11"/>
+    <sheet name="ExistingCapacitySchedule" sheetId="12" r:id="rId12"/>
+    <sheet name="WasteChpEfficiency" sheetId="13" r:id="rId13"/>
+    <sheet name="WasteAvailability" sheetId="14" r:id="rId14"/>
+    <sheet name="ExtremeEvents" sheetId="15" r:id="rId15"/>
+    <sheet name="ExtremeEventControl" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={463AE1AF-51B7-4233-AAAB-621DF3E70CA1}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{463AE1AF-51B7-4233-AAAB-621DF3E70CA1}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    SEK/tCO2
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
   <si>
     <t>parameter</t>
   </si>
@@ -84,6 +111,9 @@
     <t>elec_taxes_levies</t>
   </si>
   <si>
+    <t>n_typical_weeks</t>
+  </si>
+  <si>
     <t>technology</t>
   </si>
   <si>
@@ -114,9 +144,6 @@
     <t>lifetime_new</t>
   </si>
   <si>
-    <t>lifetime_initial</t>
-  </si>
-  <si>
     <t>Waste_CHP</t>
   </si>
   <si>
@@ -162,18 +189,6 @@
     <t>LowTempSources_HeatPump</t>
   </si>
   <si>
-    <t>year_1[MW]</t>
-  </si>
-  <si>
-    <t>year_2[MW]</t>
-  </si>
-  <si>
-    <t>year_3[MW]</t>
-  </si>
-  <si>
-    <t>year_4[MW]</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -261,43 +276,22 @@
     <t>to_low</t>
   </si>
   <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>cop_multiplier</t>
+  </si>
+  <si>
+    <t>High Temperature</t>
+  </si>
+  <si>
+    <t>Low Temperature</t>
+  </si>
+  <si>
     <t>probability</t>
   </si>
   <si>
-    <t>year_1[SEK/tCO2]</t>
-  </si>
-  <si>
-    <t>year_2[SEK/tCO2]</t>
-  </si>
-  <si>
-    <t>year_3[SEK/tCO2]</t>
-  </si>
-  <si>
-    <t>year_4[SEK/tCO2]</t>
-  </si>
-  <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>cop_multiplier</t>
-  </si>
-  <si>
-    <t>High Temperature</t>
-  </si>
-  <si>
-    <t>Low Temperature</t>
-  </si>
-  <si>
-    <t>year_1</t>
-  </si>
-  <si>
-    <t>year_2</t>
-  </si>
-  <si>
-    <t>year_3</t>
-  </si>
-  <si>
-    <t>year_4</t>
+    <t>demand_multiplier</t>
   </si>
   <si>
     <t>elec_price_multiplier</t>
@@ -309,65 +303,59 @@
     <t>normal</t>
   </si>
   <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal - baseline conditions  </t>
+  </si>
+  <si>
     <t>demand_surge</t>
   </si>
   <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Climate stress - more severe winters (20% higher average demand)</t>
+  </si>
+  <si>
     <t>price_spike</t>
   </si>
   <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>Energy crisis  -  high electricity prices (2x average)</t>
+  </si>
+  <si>
     <t>dc_outage</t>
   </si>
   <si>
-    <t>0.94</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal - baseline conditions  </t>
-  </si>
-  <si>
-    <t>Climate stress - more severe winters (20% higher average demand)</t>
-  </si>
-  <si>
-    <t>Energy crisis  -  high electricity prices (2x average)</t>
-  </si>
-  <si>
     <t>Data center supply distruption  - complete unavailability</t>
   </si>
   <si>
     <t>enable_extreme_events</t>
   </si>
   <si>
+    <t>Master switch to enable/disable extreme event modeling</t>
+  </si>
+  <si>
     <t>apply_to_year</t>
   </si>
   <si>
-    <t>Master switch to enable/disable extreme event modeling</t>
-  </si>
-  <si>
     <t>Which model year to apply extreme events</t>
-  </si>
-  <si>
-    <t>demand_multiplier</t>
-  </si>
-  <si>
-    <t>0.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,8 +371,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +409,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -428,13 +440,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,6 +468,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Kök, Ali" id="{C2436723-866E-4411-853D-B25A87398B35}" userId="S::ali.koek@tuwien.ac.at::cf6fa925-1299-4444-9ac8-ff6284848d57" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -747,18 +771,27 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2025-12-02T14:36:29.70" personId="{C2436723-866E-4411-853D-B25A87398B35}" id="{463AE1AF-51B7-4233-AAAB-621DF3E70CA1}">
+    <text xml:space="preserve">SEK/tCO2
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590D77B-7759-431A-924A-4D4114C0C169}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -777,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -841,6 +874,14 @@
       </c>
       <c r="C8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -849,38 +890,55 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916A681A-3E86-4F06-B784-91FE6167CDD3}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2030</v>
+      </c>
+      <c r="F1">
+        <v>2035</v>
+      </c>
+      <c r="G1">
+        <v>2040</v>
+      </c>
+      <c r="H1">
+        <v>2045</v>
+      </c>
+      <c r="I1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -888,19 +946,49 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>1.04</v>
+      </c>
+      <c r="F2">
+        <v>1.06</v>
+      </c>
+      <c r="G2">
+        <v>1.08</v>
+      </c>
+      <c r="H2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I2">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>106</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.9</v>
+      </c>
+      <c r="F3">
+        <v>0.875</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+      <c r="H3">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="I3">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -909,7 +997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22286C85-1058-4683-BC8D-55516C17C647}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -920,10 +1008,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>73</v>
@@ -934,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -945,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -957,11 +1045,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145D0F8-96F7-4B36-9ED7-5DAF3228EE46}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -969,24 +1057,30 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2023</v>
+      </c>
+      <c r="C1">
+        <v>2030</v>
+      </c>
+      <c r="D1">
+        <v>2035</v>
+      </c>
+      <c r="E1">
+        <v>2040</v>
+      </c>
+      <c r="F1">
+        <v>2045</v>
+      </c>
+      <c r="G1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1002,16 +1096,22 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3">
-        <v>192.71</v>
+        <v>275</v>
       </c>
       <c r="C3">
-        <v>16.600000000000001</v>
+        <v>83</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1019,8 +1119,14 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1036,8 +1142,14 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1045,33 +1157,45 @@
         <v>220</v>
       </c>
       <c r="C5">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6">
-        <v>517.29</v>
+        <v>522</v>
       </c>
       <c r="C6">
-        <v>444.3</v>
+        <v>490</v>
       </c>
       <c r="D6">
-        <v>227.7</v>
+        <v>436</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+      <c r="F6">
+        <v>207</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1087,25 +1211,37 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8">
-        <v>314.57</v>
+        <v>320</v>
       </c>
       <c r="C8">
-        <v>78</v>
+        <v>243</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1113,46 +1249,64 @@
         <v>185</v>
       </c>
       <c r="C9">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10">
-        <v>1702.14</v>
+        <v>1714</v>
       </c>
       <c r="C10">
-        <v>861.2</v>
+        <v>1540</v>
       </c>
       <c r="D10">
-        <v>56</v>
+        <v>783</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C11">
-        <v>274.5</v>
+        <v>320</v>
       </c>
       <c r="D11">
-        <v>55.9</v>
+        <v>286</v>
       </c>
       <c r="E11">
+        <v>160</v>
+      </c>
+      <c r="F11">
+        <v>27</v>
+      </c>
+      <c r="G11">
         <v>0</v>
       </c>
     </row>
@@ -1162,39 +1316,53 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF04874-5E52-4CAF-80BF-0F4F010E9C18}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2023</v>
+      </c>
+      <c r="B1">
+        <v>2030</v>
+      </c>
+      <c r="C1">
+        <v>2035</v>
+      </c>
+      <c r="D1">
+        <v>2040</v>
+      </c>
+      <c r="E1">
+        <v>2045</v>
+      </c>
+      <c r="F1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.81120000000000003</v>
+        <v>0.9</v>
       </c>
       <c r="B2">
-        <v>0.63560000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="C2">
-        <v>0.53320000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="D2">
-        <v>0.49769999999999998</v>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E2">
+        <v>0.53</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1203,39 +1371,53 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA441E4D-3EA7-459F-85DE-ECA5E8A27D8A}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>7657579.3700000001</v>
-      </c>
-      <c r="B2">
-        <v>5474361.1100000003</v>
-      </c>
-      <c r="C2">
-        <v>3731500</v>
-      </c>
-      <c r="D2">
-        <v>3034115.53</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2023</v>
+      </c>
+      <c r="B1">
+        <v>2030</v>
+      </c>
+      <c r="C1">
+        <v>2035</v>
+      </c>
+      <c r="D1">
+        <v>2040</v>
+      </c>
+      <c r="E1">
+        <v>2045</v>
+      </c>
+      <c r="F1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
+        <v>8547.2222222222226</v>
+      </c>
+      <c r="B2" s="9">
+        <v>6524.4444444444443</v>
+      </c>
+      <c r="C2" s="9">
+        <v>5303.6111111111113</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4429.7222222222217</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3637.5</v>
+      </c>
+      <c r="F2" s="9">
+        <v>3034.1155256428815</v>
       </c>
     </row>
   </sheetData>
@@ -1244,7 +1426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0160E0F-AD26-48ED-8931-1C59DFE62250}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
@@ -1263,30 +1445,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1298,18 +1480,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1318,15 +1500,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1338,15 +1520,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1358,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1367,11 +1549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4035866-F30E-4239-8029-E32D08CAEEBA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1387,29 +1569,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1418,11 +1600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B221ABC6-770B-4F46-8362-7A6F0CE97577}">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1430,44 +1612,42 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1498,11 +1678,8 @@
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1533,11 +1710,8 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1568,11 +1742,8 @@
       <c r="J4">
         <v>2</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1603,11 +1774,8 @@
       <c r="J5">
         <v>3</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1638,11 +1806,8 @@
       <c r="J6">
         <v>3</v>
       </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1673,11 +1838,8 @@
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1708,11 +1870,8 @@
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1743,11 +1902,8 @@
       <c r="J9">
         <v>2</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1778,11 +1934,8 @@
       <c r="J10">
         <v>2</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1812,9 +1965,6 @@
       </c>
       <c r="J11">
         <v>2</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1823,33 +1973,42 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420D5219-3D62-48D2-B079-889AEB0D6350}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2023</v>
+      </c>
+      <c r="C1">
+        <v>2030</v>
+      </c>
+      <c r="D1">
+        <v>2035</v>
+      </c>
+      <c r="E1">
+        <v>2040</v>
+      </c>
+      <c r="F1">
+        <v>2045</v>
+      </c>
+      <c r="G1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1865,8 +2024,14 @@
       <c r="E2">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1882,8 +2047,14 @@
       <c r="E3">
         <v>400</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1899,8 +2070,14 @@
       <c r="E4">
         <v>900</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>900</v>
+      </c>
+      <c r="G4">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1916,8 +2093,14 @@
       <c r="E5">
         <v>400</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1933,8 +2116,14 @@
       <c r="E6">
         <v>900</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>900</v>
+      </c>
+      <c r="G6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1950,8 +2139,14 @@
       <c r="E7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1967,8 +2162,14 @@
       <c r="E8">
         <v>500</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>500</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1984,8 +2185,14 @@
       <c r="E9">
         <v>365</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>365</v>
+      </c>
+      <c r="G9">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2001,8 +2208,14 @@
       <c r="E10">
         <v>250</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>250</v>
+      </c>
+      <c r="G10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2018,10 +2231,16 @@
       <c r="E11">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>95</v>
+      </c>
+      <c r="G11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -2033,6 +2252,12 @@
         <v>2000</v>
       </c>
       <c r="E12">
+        <v>2000</v>
+      </c>
+      <c r="F12">
+        <v>2000</v>
+      </c>
+      <c r="G12">
         <v>2000</v>
       </c>
     </row>
@@ -2042,7 +2267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E078A6-3DE3-4FBD-B546-0DA5EF096AA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2052,7 +2277,7 @@
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2065,7 +2290,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>400</v>
@@ -2073,7 +2298,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2081,7 +2306,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2089,7 +2314,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>0.95</v>
@@ -2097,7 +2322,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>0.02</v>
@@ -2105,7 +2330,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0.25</v>
@@ -2113,7 +2338,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>0.25</v>
@@ -2121,7 +2346,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2129,7 +2354,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>1000</v>
@@ -2137,7 +2362,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2149,7 +2374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C4674D-613B-47DC-95EC-A125610F3DBD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2158,10 +2383,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2207,7 +2432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03C60C6-D733-44AF-9BC0-050CCF024BCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2216,10 +2441,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2452,11 +2677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE8A0B0-FF39-49E0-ADEA-C8C600021327}">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2472,25 +2697,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -2498,13 +2723,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1">
         <v>2023</v>
       </c>
       <c r="D2" s="1">
-        <v>-1260</v>
+        <v>-126</v>
       </c>
       <c r="E2" s="1">
         <v>2012.4</v>
@@ -2521,13 +2746,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4">
         <v>2023</v>
       </c>
       <c r="D3" s="4">
-        <v>-1260</v>
+        <v>-126</v>
       </c>
       <c r="E3" s="4">
         <v>1548</v>
@@ -2544,22 +2769,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1">
         <v>2023</v>
       </c>
       <c r="D4" s="1">
-        <v>-1260</v>
+        <v>-126</v>
       </c>
       <c r="E4" s="1">
         <v>1083.5999999999999</v>
       </c>
       <c r="F4" s="1">
-        <v>163.79999999999998</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="G4" s="1">
-        <v>450.79999999999995</v>
+        <v>450.8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2567,19 +2792,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2">
         <v>2030</v>
       </c>
       <c r="D5" s="2">
-        <v>-1599</v>
+        <v>-160</v>
       </c>
       <c r="E5" s="2">
-        <v>2260.7000000000003</v>
+        <v>2260.6999999999998</v>
       </c>
       <c r="F5" s="2">
-        <v>341.90000000000003</v>
+        <v>341.9</v>
       </c>
       <c r="G5" s="2">
         <v>941.2</v>
@@ -2590,13 +2815,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4">
         <v>2030</v>
       </c>
       <c r="D6" s="4">
-        <v>-1599</v>
+        <v>-160</v>
       </c>
       <c r="E6" s="4">
         <v>1739</v>
@@ -2613,13 +2838,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2">
         <v>2030</v>
       </c>
       <c r="D7" s="2">
-        <v>-1599</v>
+        <v>-160</v>
       </c>
       <c r="E7" s="2">
         <v>1217.3</v>
@@ -2628,7 +2853,7 @@
         <v>184.1</v>
       </c>
       <c r="G7" s="2">
-        <v>506.79999999999995</v>
+        <v>506.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2636,22 +2861,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="D8" s="3">
-        <v>-1987</v>
+        <v>-183</v>
       </c>
       <c r="E8" s="3">
-        <v>2676.7000000000003</v>
+        <f>E9*1.3</f>
+        <v>2462.2000000000003</v>
       </c>
       <c r="F8" s="3">
-        <v>403</v>
+        <f t="shared" ref="F8:G8" si="0">F9*1.3</f>
+        <v>369.2</v>
       </c>
       <c r="G8" s="3">
-        <v>1114.1000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1024.4000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2659,22 +2887,22 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C9" s="4">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="D9" s="4">
-        <v>-1987</v>
+        <v>-183</v>
       </c>
       <c r="E9" s="4">
-        <v>2059</v>
+        <v>1894</v>
       </c>
       <c r="F9" s="4">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="G9" s="4">
-        <v>857</v>
+        <v>788</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2682,45 +2910,48 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3">
+        <v>2035</v>
+      </c>
+      <c r="D10" s="3">
+        <v>-183</v>
+      </c>
+      <c r="E10" s="3">
+        <f>E9*0.7</f>
+        <v>1325.8</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ref="F10:G10" si="1">F9*0.7</f>
+        <v>198.79999999999998</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="1"/>
+        <v>551.59999999999991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="6">
         <v>2040</v>
       </c>
-      <c r="D10" s="3">
-        <v>-1987</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1441.3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>217</v>
-      </c>
-      <c r="G10" s="3">
-        <v>599.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11">
-        <v>2050</v>
-      </c>
-      <c r="D11">
-        <v>-2278</v>
-      </c>
-      <c r="E11">
-        <v>3168.1</v>
-      </c>
-      <c r="F11">
-        <v>477.1</v>
-      </c>
-      <c r="G11">
-        <v>1319.5</v>
+      <c r="D11" s="6">
+        <v>-199</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2676.7</v>
+      </c>
+      <c r="F11" s="6">
+        <v>403</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1114.0999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2728,44 +2959,188 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C12" s="4">
+        <v>2040</v>
+      </c>
+      <c r="D12" s="4">
+        <v>-199</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2059</v>
+      </c>
+      <c r="F12" s="4">
+        <v>310</v>
+      </c>
+      <c r="G12" s="4">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2040</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-199</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1441.3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>217</v>
+      </c>
+      <c r="G13" s="6">
+        <v>599.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2045</v>
+      </c>
+      <c r="D14" s="7">
+        <v>-224</v>
+      </c>
+      <c r="E14" s="7">
+        <f>E15*1.3</f>
+        <v>2910.7000000000003</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" ref="F14:G14" si="2">F15*1.3</f>
+        <v>439.40000000000003</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="2"/>
+        <v>1211.6000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2045</v>
+      </c>
+      <c r="D15" s="4">
+        <v>-224</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2239</v>
+      </c>
+      <c r="F15" s="4">
+        <v>338</v>
+      </c>
+      <c r="G15" s="4">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>3</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2045</v>
+      </c>
+      <c r="D16" s="7">
+        <v>-224</v>
+      </c>
+      <c r="E16" s="7">
+        <f>E15*0.7</f>
+        <v>1567.3</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" ref="F16:G16" si="3">F15*0.7</f>
+        <v>236.6</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="3"/>
+        <v>652.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>1</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="8">
         <v>2050</v>
       </c>
-      <c r="D12" s="4">
-        <v>-2278</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D17" s="8">
+        <v>-228</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3168.1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>477.1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1319.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2050</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-228</v>
+      </c>
+      <c r="E18" s="4">
         <v>2437</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F18" s="4">
         <v>367</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G18" s="4">
         <v>1015</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13">
+      <c r="B19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="8">
         <v>2050</v>
       </c>
-      <c r="D13">
-        <v>-2278</v>
-      </c>
-      <c r="E13">
-        <v>1705.8999999999999</v>
-      </c>
-      <c r="F13">
+      <c r="D19" s="8">
+        <v>-228</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1705.9</v>
+      </c>
+      <c r="F19" s="8">
         <v>256.89999999999998</v>
       </c>
-      <c r="G13">
+      <c r="G19" s="8">
         <v>710.5</v>
       </c>
     </row>
@@ -2775,7 +3150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879CF66E-0559-4CA6-9CC7-E6C1E475771D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="250" workbookViewId="0">
@@ -2786,21 +3161,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>0.9</v>
@@ -2814,7 +3189,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -2828,7 +3203,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>0.01</v>
@@ -2846,33 +3221,43 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51FC39B-AAD9-4476-8BBF-DA36EB745D6A}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2023</v>
+      </c>
+      <c r="B1">
+        <v>2030</v>
+      </c>
+      <c r="C1">
+        <v>2035</v>
+      </c>
+      <c r="D1">
+        <v>2040</v>
+      </c>
+      <c r="E1">
+        <v>2045</v>
+      </c>
+      <c r="F1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1500</v>
       </c>
@@ -2880,13 +3265,22 @@
         <v>1900</v>
       </c>
       <c r="C2">
+        <f>AVERAGE(B2,D2)</f>
+        <v>2100</v>
+      </c>
+      <c r="D2">
         <v>2300</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <f>AVERAGE(D2,F2)</f>
+        <v>2515</v>
+      </c>
+      <c r="F2">
         <v>2730</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement technology-specific, year-varying heat pump COPs
Replace single COP multiplier with detailed COP trajectories per heat pump
technology, temperature scenario, and calendar year. Low-temp DH scenario
uses improving COPs from HeatPumpCOP sheet; High-temp DH uses constant 2023 values.
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF1C899-01B6-4747-A846-150BBD65C624}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5491ED-59E0-48CF-AD67-E8A03F008577}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,13 @@
     <sheet name="EnergyTransitions" sheetId="8" r:id="rId8"/>
     <sheet name="CarbonTrajectory" sheetId="9" r:id="rId9"/>
     <sheet name="TemperatureScenarios" sheetId="10" r:id="rId10"/>
-    <sheet name="TemperatureProbabilities" sheetId="11" r:id="rId11"/>
-    <sheet name="ExistingCapacitySchedule" sheetId="12" r:id="rId12"/>
-    <sheet name="WasteChpEfficiency" sheetId="13" r:id="rId13"/>
-    <sheet name="WasteAvailability" sheetId="14" r:id="rId14"/>
-    <sheet name="ExtremeEvents" sheetId="15" r:id="rId15"/>
-    <sheet name="ExtremeEventControl" sheetId="16" r:id="rId16"/>
+    <sheet name="HeatPumpCOP" sheetId="17" r:id="rId11"/>
+    <sheet name="TemperatureProbabilities" sheetId="11" r:id="rId12"/>
+    <sheet name="ExistingCapacitySchedule" sheetId="12" r:id="rId13"/>
+    <sheet name="WasteChpEfficiency" sheetId="13" r:id="rId14"/>
+    <sheet name="WasteAvailability" sheetId="14" r:id="rId15"/>
+    <sheet name="ExtremeEvents" sheetId="15" r:id="rId16"/>
+    <sheet name="ExtremeEventControl" sheetId="16" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,8 +67,44 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4D02342A-FBE5-4DB6-9C04-00FA89B0D8C7}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4D02342A-FBE5-4DB6-9C04-00FA89B0D8C7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changes in the annual demand in the temp scenarios</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7703EBF0-E384-487A-8AB0-BC9525DE85E7}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7703EBF0-E384-487A-8AB0-BC9525DE85E7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changes in the COPs in the low temp scenario</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
   <si>
     <t>parameter</t>
   </si>
@@ -277,9 +314,6 @@
   </si>
   <si>
     <t>scenario</t>
-  </si>
-  <si>
-    <t>cop_multiplier</t>
   </si>
   <si>
     <t>High Temperature</t>
@@ -780,6 +814,22 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2025-12-04T09:50:54.03" personId="{C2436723-866E-4411-853D-B25A87398B35}" id="{4D02342A-FBE5-4DB6-9C04-00FA89B0D8C7}">
+    <text>Changes in the annual demand in the temp scenarios</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2025-12-04T09:50:08.69" personId="{C2436723-866E-4411-853D-B25A87398B35}" id="{7703EBF0-E384-487A-8AB0-BC9525DE85E7}">
+    <text>Changes in the COPs in the low temp scenario</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
@@ -890,113 +940,238 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
-        <v>70</v>
+      <c r="C1">
+        <v>2023</v>
       </c>
       <c r="D1">
-        <v>2023</v>
+        <v>2030</v>
       </c>
       <c r="E1">
-        <v>2030</v>
+        <v>2035</v>
       </c>
       <c r="F1">
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="G1">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="H1">
-        <v>2045</v>
-      </c>
-      <c r="I1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="E2">
-        <v>1.04</v>
+        <v>1.06</v>
       </c>
       <c r="F2">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
       <c r="G2">
-        <v>1.08</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I2">
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
-        <v>0.9</v>
+        <v>0.875</v>
       </c>
       <c r="F3">
-        <v>0.875</v>
+        <v>0.85</v>
       </c>
       <c r="G3">
-        <v>0.85</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="H3">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="I3">
         <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A2409B-616B-4929-9692-74AC98DC6CF7}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2023</v>
+      </c>
+      <c r="C1">
+        <v>2030</v>
+      </c>
+      <c r="D1">
+        <v>2035</v>
+      </c>
+      <c r="E1">
+        <v>2040</v>
+      </c>
+      <c r="F1">
+        <v>2045</v>
+      </c>
+      <c r="G1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>6.2</v>
+      </c>
+      <c r="G2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>3.6</v>
+      </c>
+      <c r="C3">
+        <v>4.3</v>
+      </c>
+      <c r="D3">
+        <v>4.3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5.5</v>
+      </c>
+      <c r="G3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>3.7</v>
+      </c>
+      <c r="C4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>4.8</v>
+      </c>
+      <c r="F4">
+        <v>5.3</v>
+      </c>
+      <c r="G4">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>3.6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G5">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1014,7 +1189,7 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1022,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -1033,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -1044,7 +1219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1315,7 +1490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1370,7 +1545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1425,7 +1600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1448,16 +1623,16 @@
         <v>69</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>56</v>
@@ -1465,10 +1640,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" t="s">
-        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1480,18 +1655,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1500,15 +1675,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1520,15 +1695,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
         <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1540,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1574,24 +1749,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1603,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" activeCellId="3" sqref="A4 A9 A10 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3224,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add units to Excel parameter sheets and flexible column parsing
- Add unit annotations to all Excel sheets for documentation
- Implement flexible column name matching to handle unit suffixes
- Load time-varying emission factors from WasteChpEfficiency sheet
- Update parameter loading for CapacityLimits, TemperatureScenarios,
  ExistingCapacitySchedule, HeatPumpCOP, and ExtremeEvents sheets
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="319" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5491ED-59E0-48CF-AD67-E8A03F008577}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C6C00F-AE67-491F-8A6B-A14C943D6930}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-1230" windowWidth="25820" windowHeight="13900" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>parameter</t>
   </si>
@@ -383,13 +383,70 @@
   </si>
   <si>
     <t>Which model year to apply extreme events</t>
+  </si>
+  <si>
+    <t>emission_factor</t>
+  </si>
+  <si>
+    <t>efficiency [-]</t>
+  </si>
+  <si>
+    <t>emission_factor [tCO2/MWh]</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
+    <t>model years</t>
+  </si>
+  <si>
+    <t>SEK/MWh/year</t>
+  </si>
+  <si>
+    <t>[1/day]</t>
+  </si>
+  <si>
+    <t>model periods</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>carbon_price [SEK/tCO2]</t>
+  </si>
+  <si>
+    <t>availability [GWh/year]</t>
+  </si>
+  <si>
+    <t>technology [MW_th, MWh for storage]</t>
+  </si>
+  <si>
+    <t>technology [MW_th]</t>
+  </si>
+  <si>
+    <t>probability [-]</t>
+  </si>
+  <si>
+    <t>demand_multiplier [-]</t>
+  </si>
+  <si>
+    <t>elec_price_multiplier [-]</t>
+  </si>
+  <si>
+    <t>dc_availability [-]</t>
+  </si>
+  <si>
+    <t>technology (COP [-])</t>
+  </si>
+  <si>
+    <t>description (demand_multiplier [-])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -404,12 +461,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -844,7 +895,7 @@
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -863,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -877,15 +928,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -896,15 +950,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -915,7 +972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -926,12 +983,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
         <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -953,12 +1013,12 @@
     <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C1">
         <v>2023</v>
@@ -979,7 +1039,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1005,7 +1065,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1041,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A2409B-616B-4929-9692-74AC98DC6CF7}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1050,9 +1110,9 @@
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -1073,7 +1133,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1096,7 +1156,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1119,7 +1179,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1142,7 +1202,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1181,7 +1241,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1192,7 +1252,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1203,7 +1263,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1232,9 +1292,9 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -1255,7 +1315,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1301,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1324,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1347,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1370,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1393,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1416,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1439,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1462,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1492,52 +1552,84 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.9140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:7" dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>2023</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>2030</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2035</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2040</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2045</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:7" dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2">
         <v>0.9</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.71</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.62</v>
       </c>
-      <c r="D2">
-        <v>0.56999999999999995</v>
-      </c>
       <c r="E2">
+        <v>0.57</v>
+      </c>
+      <c r="F2">
         <v>0.53</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>0.324</v>
+      </c>
+      <c r="C3">
+        <v>0.27</v>
+      </c>
+      <c r="D3">
+        <v>0.23</v>
+      </c>
+      <c r="E3">
+        <v>0.205</v>
+      </c>
+      <c r="F3">
+        <v>0.176</v>
+      </c>
+      <c r="G3">
+        <v>0.151</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1639,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -1555,44 +1647,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:7" dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>2023</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>2030</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2035</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2040</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2045</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>8547.2222222222226</v>
-      </c>
-      <c r="B2" s="9">
-        <v>6524.4444444444443</v>
-      </c>
-      <c r="C2" s="9">
-        <v>5303.6111111111113</v>
-      </c>
-      <c r="D2" s="9">
-        <v>4429.7222222222217</v>
-      </c>
-      <c r="E2" s="9">
+    <row r="2" spans="1:7" dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>8547.22</v>
+      </c>
+      <c r="C2">
+        <v>6524.44</v>
+      </c>
+      <c r="D2">
+        <v>5303.61</v>
+      </c>
+      <c r="E2">
+        <v>4429.72</v>
+      </c>
+      <c r="F2">
         <v>3637.5</v>
       </c>
-      <c r="F2" s="9">
-        <v>3034.1155256428815</v>
+      <c r="G2">
+        <v>3034.12</v>
       </c>
     </row>
   </sheetData>
@@ -1618,27 +1716,27 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" dyDescent="0.35">
+      <c r="A1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" dyDescent="0.35">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1658,7 +1756,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" dyDescent="0.35">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1678,7 +1776,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" dyDescent="0.35">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1698,7 +1796,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1736,7 +1834,7 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1845,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" dyDescent="0.35">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1758,7 +1856,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" dyDescent="0.35">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1790,7 +1888,7 @@
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1822,7 +1920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1854,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1950,7 +2048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1982,7 +2080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2014,7 +2112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2046,7 +2144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2078,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2110,7 +2208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2160,9 +2258,9 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -2183,7 +2281,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2206,7 +2304,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2229,7 +2327,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2252,7 +2350,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2275,7 +2373,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2298,7 +2396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2321,7 +2419,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2344,7 +2442,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2367,7 +2465,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2390,7 +2488,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2413,7 +2511,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2443,7 +2541,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -2455,92 +2553,125 @@
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2">
         <v>400</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
       <c r="B7">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
       <c r="B8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
       <c r="B11">
         <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2552,11 +2683,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -2564,7 +2697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2705,7 @@
         <v>0.34735402116783071</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2580,12 +2713,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2593,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2614,7 +2747,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2622,7 +2755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" dyDescent="0.35">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -2630,7 +2763,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" dyDescent="0.35">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -2638,7 +2771,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" dyDescent="0.35">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -2646,7 +2779,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" dyDescent="0.35">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2654,7 +2787,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" dyDescent="0.35">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -2662,7 +2795,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" dyDescent="0.35">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -2670,7 +2803,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" dyDescent="0.35">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -2678,7 +2811,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" dyDescent="0.35">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -2686,7 +2819,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" dyDescent="0.35">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -2694,7 +2827,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" dyDescent="0.35">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -2702,7 +2835,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" dyDescent="0.35">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -2710,7 +2843,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" dyDescent="0.35">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -2718,7 +2851,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" dyDescent="0.35">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -2726,7 +2859,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" dyDescent="0.35">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -2734,7 +2867,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" dyDescent="0.35">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -2742,7 +2875,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" dyDescent="0.35">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -2750,7 +2883,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" dyDescent="0.35">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -2758,7 +2891,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" dyDescent="0.35">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -2766,7 +2899,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" dyDescent="0.35">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -2774,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" dyDescent="0.35">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -2782,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" dyDescent="0.35">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -2790,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" dyDescent="0.35">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -2798,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" dyDescent="0.35">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -2806,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" dyDescent="0.35">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -2814,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" dyDescent="0.35">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -2822,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" dyDescent="0.35">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -2830,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" dyDescent="0.35">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -2838,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" dyDescent="0.35">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -2870,7 +3003,7 @@
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -2893,11 +3026,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="1">
         <v>62</v>
       </c>
       <c r="C2" s="1">
@@ -2916,11 +3049,11 @@
         <v>837.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C3" s="4">
@@ -2939,11 +3072,11 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s" s="1">
         <v>64</v>
       </c>
       <c r="C4" s="1">
@@ -2962,11 +3095,11 @@
         <v>450.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s" s="2">
         <v>62</v>
       </c>
       <c r="C5" s="2">
@@ -2985,11 +3118,11 @@
         <v>941.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C6" s="4">
@@ -3008,11 +3141,11 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s" s="2">
         <v>64</v>
       </c>
       <c r="C7" s="2">
@@ -3031,11 +3164,11 @@
         <v>506.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s" s="3">
         <v>62</v>
       </c>
       <c r="C8" s="3">
@@ -3049,7 +3182,7 @@
         <v>2462.2000000000003</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ref="F8:G8" si="0">F9*1.3</f>
+        <f t="shared" si="0" ref="F8:G8">F9*1.3</f>
         <v>369.2</v>
       </c>
       <c r="G8" s="3">
@@ -3057,11 +3190,11 @@
         <v>1024.4000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C9" s="4">
@@ -3080,11 +3213,11 @@
         <v>788</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" dyDescent="0.35">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s" s="3">
         <v>64</v>
       </c>
       <c r="C10" s="3">
@@ -3098,7 +3231,7 @@
         <v>1325.8</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ref="F10:G10" si="1">F9*0.7</f>
+        <f t="shared" si="1" ref="F10:G10">F9*0.7</f>
         <v>198.79999999999998</v>
       </c>
       <c r="G10" s="3">
@@ -3106,11 +3239,11 @@
         <v>551.59999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s" s="6">
         <v>62</v>
       </c>
       <c r="C11" s="6">
@@ -3129,11 +3262,11 @@
         <v>1114.0999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C12" s="4">
@@ -3152,11 +3285,11 @@
         <v>857</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" dyDescent="0.35">
       <c r="A13" s="6">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s" s="6">
         <v>64</v>
       </c>
       <c r="C13" s="6">
@@ -3175,11 +3308,11 @@
         <v>599.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" dyDescent="0.35">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s" s="7">
         <v>62</v>
       </c>
       <c r="C14" s="7">
@@ -3193,7 +3326,7 @@
         <v>2910.7000000000003</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" ref="F14:G14" si="2">F15*1.3</f>
+        <f t="shared" si="2" ref="F14:G14">F15*1.3</f>
         <v>439.40000000000003</v>
       </c>
       <c r="G14" s="7">
@@ -3201,11 +3334,11 @@
         <v>1211.6000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C15" s="4">
@@ -3224,11 +3357,11 @@
         <v>932</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" dyDescent="0.35">
       <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" t="s" s="7">
         <v>64</v>
       </c>
       <c r="C16" s="7">
@@ -3242,7 +3375,7 @@
         <v>1567.3</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" ref="F16:G16" si="3">F15*0.7</f>
+        <f t="shared" si="3" ref="F16:G16">F15*0.7</f>
         <v>236.6</v>
       </c>
       <c r="G16" s="7">
@@ -3250,11 +3383,11 @@
         <v>652.4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" dyDescent="0.35">
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s" s="8">
         <v>62</v>
       </c>
       <c r="C17" s="8">
@@ -3273,11 +3406,11 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s" s="4">
         <v>63</v>
       </c>
       <c r="C18" s="4">
@@ -3296,11 +3429,11 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" dyDescent="0.35">
       <c r="A19" s="8">
         <v>3</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s" s="8">
         <v>64</v>
       </c>
       <c r="C19" s="8">
@@ -3334,22 +3467,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s" s="5">
         <v>66</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s" s="5">
         <v>67</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s" s="5">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" dyDescent="0.35">
+      <c r="A2" t="s" s="5">
         <v>62</v>
       </c>
       <c r="B2">
@@ -3362,8 +3495,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" dyDescent="0.35">
+      <c r="A3" t="s" s="5">
         <v>63</v>
       </c>
       <c r="B3">
@@ -3376,8 +3509,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" dyDescent="0.35">
+      <c r="A4" t="s" s="5">
         <v>64</v>
       </c>
       <c r="B4">
@@ -3397,7 +3530,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
@@ -3412,46 +3545,50 @@
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:7" dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>2023</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>2030</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2035</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2040</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2045</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1500</v>
+    <row r="2" spans="1:7" dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
       </c>
       <c r="B2">
-        <v>1900</v>
+        <v>1330</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(B2,D2)</f>
-        <v>2100</v>
+        <v>1581</v>
       </c>
       <c r="D2">
-        <v>2300</v>
+        <v>1789</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(D2,F2)</f>
-        <v>2515</v>
+        <v>2024</v>
       </c>
       <c r="F2">
-        <v>2730</v>
+        <v>2290</v>
+      </c>
+      <c r="G2">
+        <v>2591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add minimum load factor constraint for Waste CHP
Implements realistic waste incineration operation by requiring Waste CHP
to run at a minimum percentage of available capacity every hour.

Changes:
- Add waste_min_load_factor parameter to ModelConfig (0-1, e.g., 0.25 = 25%)
- Add constraint: u_production[:Waste_CHP] >= min_load_factor * capacity_alive
- Always feasible (satisfies SDDP relatively complete recourse requirement)

This ensures waste incineration operates as baseload, reflecting real-world
continuous operation requirements.
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C6C00F-AE67-491F-8A6B-A14C943D6930}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E9A06F-D0FF-4CFE-98D9-C2F3CDE81F9A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
   <si>
     <t>parameter</t>
   </si>
@@ -118,9 +118,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>representative model years</t>
-  </si>
-  <si>
     <t>T_years</t>
   </si>
   <si>
@@ -325,51 +322,27 @@
     <t>probability</t>
   </si>
   <si>
-    <t>demand_multiplier</t>
-  </si>
-  <si>
-    <t>elec_price_multiplier</t>
-  </si>
-  <si>
-    <t>dc_availability</t>
-  </si>
-  <si>
     <t>normal</t>
   </si>
   <si>
-    <t>0.94</t>
-  </si>
-  <si>
     <t xml:space="preserve">Normal - baseline conditions  </t>
   </si>
   <si>
     <t>demand_surge</t>
   </si>
   <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
     <t>Climate stress - more severe winters (20% higher average demand)</t>
   </si>
   <si>
     <t>price_spike</t>
   </si>
   <si>
-    <t>0.02</t>
-  </si>
-  <si>
     <t>Energy crisis  -  high electricity prices (2x average)</t>
   </si>
   <si>
     <t>dc_outage</t>
   </si>
   <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>Data center supply distruption  - complete unavailability</t>
   </si>
   <si>
@@ -385,9 +358,6 @@
     <t>Which model year to apply extreme events</t>
   </si>
   <si>
-    <t>emission_factor</t>
-  </si>
-  <si>
     <t>efficiency [-]</t>
   </si>
   <si>
@@ -440,6 +410,9 @@
   </si>
   <si>
     <t>description (demand_multiplier [-])</t>
+  </si>
+  <si>
+    <t>waste_min_load_factor</t>
   </si>
 </sst>
 </file>
@@ -525,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -535,9 +508,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -895,7 +865,7 @@
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -914,84 +884,95 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
       <c r="B4">
         <v>0.04</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>7901900</v>
       </c>
       <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
       </c>
       <c r="B6">
         <v>0.9</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>10000</v>
       </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
       </c>
       <c r="B8">
         <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1013,12 +994,12 @@
     <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C1">
         <v>2023</v>
@@ -1039,12 +1020,12 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:8" dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1065,12 +1046,12 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1110,9 +1091,9 @@
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -1133,9 +1114,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1156,9 +1137,9 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>3.6</v>
@@ -1179,9 +1160,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>3.7</v>
@@ -1202,9 +1183,9 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>3.6</v>
@@ -1241,34 +1222,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -1292,9 +1273,9 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -1315,9 +1296,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1338,9 +1319,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>275</v>
@@ -1361,32 +1342,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>37</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>38</v>
       </c>
       <c r="B5">
         <v>220</v>
@@ -1407,9 +1388,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>522</v>
@@ -1430,9 +1411,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1453,9 +1434,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>320</v>
@@ -1476,9 +1457,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>185</v>
@@ -1499,9 +1480,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>1714</v>
@@ -1522,9 +1503,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>334</v>
@@ -1554,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1563,7 +1544,7 @@
     <col min="1" max="1" width="13.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1586,9 +1567,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0.9</v>
@@ -1600,7 +1581,7 @@
         <v>0.62</v>
       </c>
       <c r="E2">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F2">
         <v>0.53</v>
@@ -1609,12 +1590,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B3">
-        <v>0.324</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="C3">
         <v>0.27</v>
@@ -1623,10 +1604,10 @@
         <v>0.23</v>
       </c>
       <c r="E3">
-        <v>0.205</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F3">
-        <v>0.176</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="G3">
         <v>0.151</v>
@@ -1647,7 +1628,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1670,12 +1651,12 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B2">
-        <v>8547.22</v>
+        <v>8547.2199999999993</v>
       </c>
       <c r="C2">
         <v>6524.44</v>
@@ -1703,7 +1684,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1716,32 +1697,32 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0.94</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1753,18 +1734,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>0.03</v>
+      </c>
+      <c r="C3">
+        <v>1.2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1773,15 +1754,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1793,15 +1774,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1813,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1834,7 +1815,7 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1842,29 +1823,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1888,41 +1869,41 @@
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>25</v>
       </c>
       <c r="B2">
         <v>330</v>
@@ -1946,15 +1927,15 @@
         <v>0.26</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>430</v>
@@ -1978,15 +1959,15 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>320</v>
@@ -2010,15 +1991,15 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>185</v>
@@ -2042,15 +2023,15 @@
         <v>0.21</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>522</v>
@@ -2074,15 +2055,15 @@
         <v>0.27</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1700</v>
@@ -2106,15 +2087,15 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>275</v>
@@ -2138,15 +2119,15 @@
         <v>0.5</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2170,15 +2151,15 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>220</v>
@@ -2202,15 +2183,15 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2234,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -2250,7 +2231,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2258,9 +2239,9 @@
     <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B1">
         <v>2023</v>
@@ -2281,9 +2262,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>-1</v>
@@ -2304,9 +2285,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:7" dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -2327,9 +2308,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -2350,9 +2331,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:7" dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -2373,9 +2354,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:7" dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -2396,9 +2377,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:7" dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -2419,9 +2400,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -2442,9 +2423,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -2465,9 +2446,9 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:7" dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -2488,9 +2469,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:7" dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -2511,9 +2492,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -2553,7 +2534,7 @@
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2564,114 +2545,114 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>43</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>44</v>
       </c>
       <c r="B5">
         <v>0.95</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.02</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>0.25</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.25</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>1000</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2689,46 +2670,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0.34735402116783071</v>
       </c>
     </row>
-    <row r="3" spans="1:2" dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2747,15 +2728,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -2763,7 +2744,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -2771,7 +2752,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -2779,7 +2760,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2787,7 +2768,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -2795,7 +2776,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -2803,7 +2784,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -2811,7 +2792,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -2819,7 +2800,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -2827,7 +2808,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -2835,7 +2816,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -2843,7 +2824,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -2851,7 +2832,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -2859,7 +2840,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -2867,7 +2848,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -2875,7 +2856,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -2883,7 +2864,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -2891,7 +2872,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -2899,7 +2880,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -2907,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -2915,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -2923,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -2931,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -2939,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -2947,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -2955,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -2963,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -2971,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -3003,35 +2984,35 @@
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="1">
-        <v>62</v>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>2023</v>
@@ -3049,12 +3030,12 @@
         <v>837.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="4">
-        <v>63</v>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="4">
         <v>2023</v>
@@ -3072,12 +3053,12 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="1">
-        <v>64</v>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C4" s="1">
         <v>2023</v>
@@ -3095,12 +3076,12 @@
         <v>450.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="2">
-        <v>62</v>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C5" s="2">
         <v>2030</v>
@@ -3118,12 +3099,12 @@
         <v>941.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" t="s" s="4">
-        <v>63</v>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C6" s="4">
         <v>2030</v>
@@ -3141,12 +3122,12 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:7" dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" t="s" s="2">
-        <v>64</v>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="2">
         <v>2030</v>
@@ -3164,12 +3145,12 @@
         <v>506.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="3">
-        <v>62</v>
+      <c r="B8" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C8" s="3">
         <v>2035</v>
@@ -3182,7 +3163,7 @@
         <v>2462.2000000000003</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0" ref="F8:G8">F9*1.3</f>
+        <f t="shared" ref="F8:G8" si="0">F9*1.3</f>
         <v>369.2</v>
       </c>
       <c r="G8" s="3">
@@ -3190,12 +3171,12 @@
         <v>1024.4000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" t="s" s="4">
-        <v>63</v>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C9" s="4">
         <v>2035</v>
@@ -3213,12 +3194,12 @@
         <v>788</v>
       </c>
     </row>
-    <row r="10" spans="1:7" dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="3">
-        <v>64</v>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C10" s="3">
         <v>2035</v>
@@ -3231,7 +3212,7 @@
         <v>1325.8</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1" ref="F10:G10">F9*0.7</f>
+        <f t="shared" ref="F10:G10" si="1">F9*0.7</f>
         <v>198.79999999999998</v>
       </c>
       <c r="G10" s="3">
@@ -3239,12 +3220,12 @@
         <v>551.59999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:7" dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="6">
-        <v>62</v>
+      <c r="B11" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C11" s="6">
         <v>2040</v>
@@ -3262,12 +3243,12 @@
         <v>1114.0999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" t="s" s="4">
-        <v>63</v>
+      <c r="B12" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C12" s="4">
         <v>2040</v>
@@ -3285,12 +3266,12 @@
         <v>857</v>
       </c>
     </row>
-    <row r="13" spans="1:7" dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>3</v>
       </c>
-      <c r="B13" t="s" s="6">
-        <v>64</v>
+      <c r="B13" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C13" s="6">
         <v>2040</v>
@@ -3308,12 +3289,12 @@
         <v>599.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" t="s" s="7">
-        <v>62</v>
+      <c r="B14" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C14" s="7">
         <v>2045</v>
@@ -3326,7 +3307,7 @@
         <v>2910.7000000000003</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="2" ref="F14:G14">F15*1.3</f>
+        <f t="shared" ref="F14:G14" si="2">F15*1.3</f>
         <v>439.40000000000003</v>
       </c>
       <c r="G14" s="7">
@@ -3334,12 +3315,12 @@
         <v>1211.6000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" t="s" s="4">
-        <v>63</v>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C15" s="4">
         <v>2045</v>
@@ -3357,12 +3338,12 @@
         <v>932</v>
       </c>
     </row>
-    <row r="16" spans="1:7" dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" t="s" s="7">
-        <v>64</v>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="C16" s="7">
         <v>2045</v>
@@ -3375,7 +3356,7 @@
         <v>1567.3</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="3" ref="F16:G16">F15*0.7</f>
+        <f t="shared" ref="F16:G16" si="3">F15*0.7</f>
         <v>236.6</v>
       </c>
       <c r="G16" s="7">
@@ -3383,12 +3364,12 @@
         <v>652.4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="8">
-        <v>62</v>
+      <c r="B17" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C17" s="8">
         <v>2050</v>
@@ -3406,12 +3387,12 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" dyDescent="0.35" s="4" customFormat="1">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" t="s" s="4">
-        <v>63</v>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C18" s="4">
         <v>2050</v>
@@ -3429,12 +3410,12 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="19" spans="1:7" dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>3</v>
       </c>
-      <c r="B19" t="s" s="8">
-        <v>64</v>
+      <c r="B19" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C19" s="8">
         <v>2050</v>
@@ -3467,23 +3448,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s" s="5">
+      <c r="C1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s" s="5">
+      <c r="D1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s" s="5">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" dyDescent="0.35">
-      <c r="A2" t="s" s="5">
-        <v>62</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B2">
         <v>0.9</v>
@@ -3495,9 +3476,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:4" dyDescent="0.35">
-      <c r="A3" t="s" s="5">
-        <v>63</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -3509,9 +3490,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:4" dyDescent="0.35">
-      <c r="A4" t="s" s="5">
-        <v>64</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="B4">
         <v>0.01</v>
@@ -3545,7 +3526,7 @@
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3568,9 +3549,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B2">
         <v>1330</v>

</xml_diff>

<commit_message>
Update model parameters for VSS analysis
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects2\AlisWorkspace\PhD\Capacity Expansion\DH-Capacity-Expansion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="11_4793946D688F12D0F753310620297A3132595CB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E9A06F-D0FF-4CFE-98D9-C2F3CDE81F9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F5B8E-A822-4356-912B-D0218C65D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>87</v>
@@ -925,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>86</v>
@@ -947,7 +947,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" activeCellId="3" sqref="A4 A9 A10 A11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1973,7 +1973,7 @@
         <v>320</v>
       </c>
       <c r="C4">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="D4">
         <v>7.4</v>

</xml_diff>

<commit_message>
Finalize model parameters for publication
</commit_message>
<xml_diff>
--- a/data/model_parameters.xlsx
+++ b/data/model_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects2\AlisWorkspace\PhD\Capacity Expansion\DH-Capacity-Expansion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuwienacat-my.sharepoint.com/personal/ali_koek_tuwien_ac_at/Documents/Desktop/PhD/Capacity Expansion/Code/DH-Capacity-Expansion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F5B8E-A822-4356-912B-D0218C65D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1875" yWindow="1875" windowWidth="12525" windowHeight="6675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelConfig" sheetId="1" r:id="rId1"/>
@@ -855,17 +855,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -887,7 +887,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -898,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -909,7 +909,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -920,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -942,7 +942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -953,7 +953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -964,7 +964,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -988,13 +988,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1086,12 +1086,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1220,9 +1220,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1268,12 +1268,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.0625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1539,12 +1539,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1623,12 +1623,12 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -1687,17 +1687,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.0625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.0625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.8125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1810,12 +1810,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1857,19 +1857,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.0625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2230,16 +2230,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.0625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -2262,7 +2260,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2285,7 +2283,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2308,7 +2306,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2331,7 +2329,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2354,7 +2352,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2377,7 +2375,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2400,7 +2398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2423,7 +2421,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2446,7 +2444,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2469,7 +2467,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2492,7 +2490,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2525,16 +2523,16 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2545,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2556,7 +2554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2567,7 +2565,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2578,7 +2576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2589,7 +2587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2622,7 +2620,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2633,7 +2631,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2644,7 +2642,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2668,9 +2666,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -2678,7 +2676,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2686,7 +2684,7 @@
         <v>0.34735402116783071</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -2694,12 +2692,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2707,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2726,9 +2724,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2736,7 +2734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -2744,7 +2742,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -2752,7 +2750,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -2760,7 +2758,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2768,7 +2766,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -2776,7 +2774,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -2784,7 +2782,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -2792,7 +2790,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -2800,7 +2798,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -2808,7 +2806,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -2816,7 +2814,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -2824,7 +2822,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -2832,7 +2830,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>2035</v>
       </c>
@@ -2840,7 +2838,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2036</v>
       </c>
@@ -2848,7 +2846,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>2037</v>
       </c>
@@ -2856,7 +2854,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2038</v>
       </c>
@@ -2864,7 +2862,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>2039</v>
       </c>
@@ -2872,7 +2870,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>2040</v>
       </c>
@@ -2880,7 +2878,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>2041</v>
       </c>
@@ -2888,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>2042</v>
       </c>
@@ -2896,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>2043</v>
       </c>
@@ -2904,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>2044</v>
       </c>
@@ -2912,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>2045</v>
       </c>
@@ -2920,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>2046</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>2047</v>
       </c>
@@ -2936,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>2048</v>
       </c>
@@ -2944,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>2049</v>
       </c>
@@ -2952,7 +2950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>2050</v>
       </c>
@@ -2973,18 +2971,18 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.8125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.3125" customWidth="1"/>
+    <col min="4" max="4" width="15.0625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3007,7 +3005,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3030,7 +3028,7 @@
         <v>837.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3053,7 +3051,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3076,7 +3074,7 @@
         <v>450.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -3099,7 +3097,7 @@
         <v>941.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -3122,7 +3120,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -3145,7 +3143,7 @@
         <v>506.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -3171,7 +3169,7 @@
         <v>1024.4000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -3194,7 +3192,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -3220,7 +3218,7 @@
         <v>551.59999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -3243,7 +3241,7 @@
         <v>1114.0999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -3266,7 +3264,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -3289,7 +3287,7 @@
         <v>599.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -3315,7 +3313,7 @@
         <v>1211.6000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -3338,7 +3336,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="7">
         <v>3</v>
       </c>
@@ -3364,7 +3362,7 @@
         <v>652.4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="8">
         <v>1</v>
       </c>
@@ -3387,7 +3385,7 @@
         <v>1319.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -3410,7 +3408,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="8">
         <v>3</v>
       </c>
@@ -3446,9 +3444,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -3476,7 +3474,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="5" t="s">
         <v>62</v>
       </c>
@@ -3490,7 +3488,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
@@ -3517,16 +3515,16 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3125" customWidth="1"/>
+    <col min="4" max="4" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.3125" customWidth="1"/>
+    <col min="6" max="6" width="15.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3549,7 +3547,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>92</v>
       </c>

</xml_diff>